<commit_message>
Atualização automática 2025-09-30 15:32:05
</commit_message>
<xml_diff>
--- a/transacoes_sap.xlsx
+++ b/transacoes_sap.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\U623373\Desktop\dic_sap\github\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="5" documentId="13_ncr:1_{50ADE3E8-72AC-4F24-B166-4BC569CD0DED}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{41DC156F-DD9E-43DD-9DE5-507F03D5D9FD}"/>
+  <xr:revisionPtr revIDLastSave="8" documentId="13_ncr:1_{50ADE3E8-72AC-4F24-B166-4BC569CD0DED}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{4979835C-367B-4B23-97F9-7A703625E091}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{77C9B20D-37FF-4BED-A8BD-96C6BDDAFD3A}"/>
   </bookViews>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="144" uniqueCount="143">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="146" uniqueCount="145">
   <si>
     <t>Descrição</t>
   </si>
@@ -468,6 +468,12 @@
   </si>
   <si>
     <t>FBL1N</t>
+  </si>
+  <si>
+    <t>Extração Saldo de Razão das Contas Resumido</t>
+  </si>
+  <si>
+    <t>ZFI127</t>
   </si>
 </sst>
 </file>
@@ -839,10 +845,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EB2CB70D-AC85-45EC-AC43-CC4E571F42B6}">
-  <dimension ref="A1:B72"/>
+  <dimension ref="A1:B73"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A60" workbookViewId="0">
-      <selection activeCell="A72" sqref="A72"/>
+      <selection activeCell="A74" sqref="A74"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="35.140625" defaultRowHeight="15"/>
@@ -1427,6 +1433,14 @@
         <v>142</v>
       </c>
     </row>
+    <row r="73" spans="1:2">
+      <c r="A73" t="s">
+        <v>143</v>
+      </c>
+      <c r="B73" t="s">
+        <v>144</v>
+      </c>
+    </row>
   </sheetData>
   <autoFilter ref="A1:B70" xr:uid="{EB2CB70D-AC85-45EC-AC43-CC4E571F42B6}"/>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
@@ -1438,6 +1452,15 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Documento" ma:contentTypeID="0x0101007D09E90CD810884BAFCAD4823A1817BA" ma:contentTypeVersion="18" ma:contentTypeDescription="Crie um novo documento." ma:contentTypeScope="" ma:versionID="a5f216c500005e767098a9ff07094546">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="04122236-30bc-4d1f-834a-a6fbe18e83f3" xmlns:ns3="46f92d61-b6ca-485f-907f-de7094f59048" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="884a8f76dfd19173da2095080af7639f" ns2:_="" ns3:_="">
     <xsd:import namespace="04122236-30bc-4d1f-834a-a6fbe18e83f3"/>
@@ -1692,15 +1715,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
@@ -1713,11 +1727,11 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{97E9F1F4-B391-4B9B-88E0-F23B13F4DC80}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{EEE0335D-9EE8-45FC-AC08-4580DB282A0C}"/>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{EEE0335D-9EE8-45FC-AC08-4580DB282A0C}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{97E9F1F4-B391-4B9B-88E0-F23B13F4DC80}"/>
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>

</xml_diff>